<commit_message>
use currency from account
</commit_message>
<xml_diff>
--- a/packages/storybook/stories/data/empty.xlsx
+++ b/packages/storybook/stories/data/empty.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20100" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20100"/>
   </bookViews>
   <sheets>
     <sheet name="accounts" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
   <si>
     <t>id</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>rrule</t>
+  </si>
+  <si>
+    <t>currencyCode</t>
   </si>
 </sst>
 </file>
@@ -503,13 +506,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,14 +547,17 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
         <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:L1" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -561,9 +567,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -619,13 +625,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -680,9 +686,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -713,9 +719,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -746,9 +752,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -770,9 +776,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>